<commit_message>
filtering and fixing scripts
</commit_message>
<xml_diff>
--- a/Data/metadata/BLEED_metadata.xlsx
+++ b/Data/metadata/BLEED_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mab/Documents/GitHub/bryozoa/magnifica/Data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0F1BD4-85AA-3D4B-9663-1A5A4E948068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADFE509-E7D0-C746-B1AE-D940063D6A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="4880" windowWidth="24840" windowHeight="13380" xr2:uid="{E0C5F101-86CA-F14A-87EC-A5BEB6242023}"/>
+    <workbookView xWindow="4300" yWindow="4880" windowWidth="26980" windowHeight="17020" xr2:uid="{E0C5F101-86CA-F14A-87EC-A5BEB6242023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1215,11 +1215,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2B02F5-F55D-814A-B99A-43E342360113}">
   <dimension ref="A1:AR28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1583,10 +1588,10 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
         <v>172</v>
-      </c>
-      <c r="B4" t="s">
-        <v>173</v>
       </c>
       <c r="C4" t="s">
         <v>174</v>
@@ -1696,10 +1701,10 @@
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
         <v>175</v>
-      </c>
-      <c r="B5" t="s">
-        <v>176</v>
       </c>
       <c r="C5" t="s">
         <v>174</v>
@@ -2166,10 +2171,10 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" t="s">
         <v>184</v>
-      </c>
-      <c r="B9" t="s">
-        <v>185</v>
       </c>
       <c r="C9" t="s">
         <v>174</v>
@@ -2285,10 +2290,10 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" t="s">
         <v>186</v>
-      </c>
-      <c r="B10" t="s">
-        <v>187</v>
       </c>
       <c r="C10" t="s">
         <v>174</v>
@@ -3824,10 +3829,10 @@
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>217</v>
+      </c>
+      <c r="B25" t="s">
         <v>216</v>
-      </c>
-      <c r="B25" t="s">
-        <v>217</v>
       </c>
       <c r="C25" t="s">
         <v>174</v>
@@ -3943,10 +3948,10 @@
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" t="s">
         <v>218</v>
-      </c>
-      <c r="B26" t="s">
-        <v>219</v>
       </c>
       <c r="C26" t="s">
         <v>174</v>
@@ -4062,10 +4067,10 @@
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>221</v>
+      </c>
+      <c r="B27" t="s">
         <v>220</v>
-      </c>
-      <c r="B27" t="s">
-        <v>221</v>
       </c>
       <c r="C27" t="s">
         <v>174</v>
@@ -4178,10 +4183,10 @@
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B28" t="s">
         <v>222</v>
-      </c>
-      <c r="B28" t="s">
-        <v>223</v>
       </c>
       <c r="C28" t="s">
         <v>174</v>

</xml_diff>